<commit_message>
Lab complete. Study on the (Level Up) part later
</commit_message>
<xml_diff>
--- a/Data/Zipcode_Demos.xlsx
+++ b/Data/Zipcode_Demos.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\Moringa_Phase_1\Course_Material\Labs\dsc-importing-data-using-pandas-lab\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45F1A72-661D-4C34-B87E-DD64ED7187DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>Average Statistics</t>
   </si>
@@ -160,8 +166,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,13 +230,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +282,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -302,6 +316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -336,9 +351,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -511,37 +527,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>10005.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>10005.799999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,7 +573,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -557,31 +581,31 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0.404</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>4.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0.396</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>0.39600000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -589,7 +613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -597,7 +621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -605,7 +629,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -613,7 +637,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -621,7 +645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -629,7 +653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -637,7 +661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -645,7 +669,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -653,7 +677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -661,7 +685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
@@ -669,7 +693,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -677,7 +701,7 @@
         <v>0.437</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -685,15 +709,15 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23">
-        <v>0.036</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -701,15 +725,15 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25">
-        <v>0.181</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>0.18099999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -717,7 +741,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -725,7 +749,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
@@ -733,7 +757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -741,7 +765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>27</v>
       </c>
@@ -749,15 +773,15 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B31">
-        <v>79.90000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>79.900000000000006</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -765,15 +789,15 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B33">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -781,15 +805,15 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B35">
-        <v>0.739</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -797,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -805,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
@@ -813,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
@@ -821,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
@@ -829,7 +853,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>38</v>
       </c>
@@ -837,15 +861,15 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B42">
-        <v>2.3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>40</v>
       </c>
@@ -853,7 +877,7 @@
         <v>0.151</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>41</v>
       </c>
@@ -861,15 +885,15 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B45">
-        <v>0.649</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>0.64900000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>43</v>
       </c>
@@ -877,7 +901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>44</v>
       </c>
@@ -885,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>45</v>
       </c>
@@ -893,7 +917,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="49" spans="1:46">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
@@ -1033,7 +1057,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:46">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>10001</v>
       </c>
@@ -1086,7 +1110,7 @@
         <v>3</v>
       </c>
       <c r="R50">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="S50">
         <v>1</v>
@@ -1104,7 +1128,7 @@
         <v>3</v>
       </c>
       <c r="X50">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="Y50">
         <v>0</v>
@@ -1158,7 +1182,7 @@
         <v>24</v>
       </c>
       <c r="AP50">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AQ50">
         <v>0</v>
@@ -1173,7 +1197,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:46">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>10002</v>
       </c>
@@ -1268,7 +1292,7 @@
         <v>33</v>
       </c>
       <c r="AF51">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -1298,7 +1322,7 @@
         <v>33</v>
       </c>
       <c r="AP51">
-        <v>0.9399999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="AQ51">
         <v>0</v>
@@ -1313,7 +1337,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:46">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>10003</v>
       </c>
@@ -1453,7 +1477,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:46">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>10004</v>
       </c>
@@ -1593,7 +1617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:46">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>10005</v>
       </c>
@@ -1733,7 +1757,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:46">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>10006</v>
       </c>
@@ -1873,7 +1897,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:46">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>10007</v>
       </c>
@@ -2013,7 +2037,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:46">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>10009</v>
       </c>
@@ -2153,7 +2177,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:46">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>10010</v>
       </c>
@@ -2293,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:46">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>10011</v>
       </c>

</xml_diff>